<commit_message>
add some new rxns
</commit_message>
<xml_diff>
--- a/dente_kinetics.xlsx
+++ b/dente_kinetics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\YandexDisk\2. Workplaces\0.1 Tomsk Polytech\02. Reactor Models\Reference Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SteamCracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="rxns" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
   <si>
     <t>E</t>
   </si>
@@ -109,6 +109,42 @@
   </si>
   <si>
     <t>137.06780078125</t>
+  </si>
+  <si>
+    <t>PROPYLENE</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>C2H4 + H2 --&gt; C2H6</t>
+  </si>
+  <si>
+    <t>ETHYLENE`</t>
+  </si>
+  <si>
+    <t>C3H6 + H2 --&gt; C3H8</t>
+  </si>
+  <si>
+    <t>C2H6 --&gt; 2 CH3*</t>
+  </si>
+  <si>
+    <t>CH3_</t>
+  </si>
+  <si>
+    <t>C3H8 --&gt;  CH3* + C2H5*</t>
+  </si>
+  <si>
+    <t>C2H5_</t>
+  </si>
+  <si>
+    <t>CH3* + H2 --&gt; C2H4 + H*</t>
+  </si>
+  <si>
+    <t>METHANE</t>
+  </si>
+  <si>
+    <t>H_</t>
   </si>
 </sst>
 </file>
@@ -145,11 +181,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -165,9 +205,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -205,7 +245,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -277,7 +317,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -427,165 +467,581 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S10"/>
+  <dimension ref="A2:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>18</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>0</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="L3" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
         <v>2</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>5</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="D4">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="J4">
         <v>4</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="M4">
         <v>3</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5">
-        <v>-1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5">
-        <v>13.9</v>
-      </c>
-      <c r="N5">
-        <f>10^M5</f>
-        <v>79432823472428.328</v>
-      </c>
-      <c r="O5">
-        <v>71</v>
-      </c>
-      <c r="P5">
-        <f>O5*4.1868</f>
-        <v>297.26279999999997</v>
-      </c>
-      <c r="Q5">
-        <f>P5*1000</f>
-        <v>297262.8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6">
-        <v>8.9</v>
-      </c>
-      <c r="N6">
-        <f>10^M6</f>
-        <v>794328234.72428453</v>
-      </c>
-      <c r="O6">
-        <v>38</v>
-      </c>
-      <c r="P6">
-        <f>O6*4.1868</f>
-        <v>159.0984</v>
-      </c>
-      <c r="Q6">
-        <f>P6*1000</f>
-        <v>159098.4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B10" t="str">
-        <f>CONCATENATE("Reaction('",B5,"', ",
-"[",D5,", ",E5,IF(COUNTA(D5:G5)=2,"]",IF(COUNTA(D5:G5)=3,CONCATENATE(", ",F5,"], "),IF(COUNTA(D5:G5)=4,CONCATENATE(", ",F5,", ",G5,"], "),NA()))),
-"[",H5,", ",I5,IF(COUNTA(D5:G5)=2,"]",IF(COUNTA(D5:G5)=3,CONCATENATE(", ",J5,"], "),IF(COUNTA(D5:G5)=4,CONCATENATE(", ",J5,", ",K5,"], "),NA()))),
-"[",H5,", ",I5,IF(COUNTA(D5:G5)=2,"]",IF(COUNTA(D5:G5)=3,CONCATENATE(", ",J5,"], "),IF(COUNTA(D5:G5)=4,CONCATENATE(", ",J5,", ",K5,"], "),NA()))),
-L5,", ",
-REPLACE(N5,FIND(",",N5),1,"."),", ",
-REPLACE(P5,FIND(",",P5),1,"."),") "
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>CONCATENATE("Reaction('",F5,"', ",
+"[",G5,", ",H5,IF(COUNTA(G5:J5)=2,"]",IF(COUNTA(G5:J5)=3,CONCATENATE(", ",I5,"], "),IF(COUNTA(G5:J5)=4,CONCATENATE(", ",I5,", ",J5,"], "),NA()))),
+"[",K5,", ",L5,IF(COUNTA(G5:J5)=2,"]",IF(COUNTA(G5:J5)=3,CONCATENATE(", ",M5,"], "),IF(COUNTA(G5:J5)=4,CONCATENATE(", ",M5,", ",N5,"], "),NA()))),
+"[",K5,", ",L5,IF(COUNTA(G5:J5)=2,"]",IF(COUNTA(G5:J5)=3,CONCATENATE(", ",M5,"], "),IF(COUNTA(G5:J5)=4,CONCATENATE(", ",M5,", ",N5,"], "),NA()))),
+O5,", ",
+REPLACE(Q5,FIND(",",Q5),1,"."),", ",
+REPLACE(S5,FIND(",",S5),1,"."),") "
 )</f>
         <v xml:space="preserve">Reaction('C2H6 --&gt; C2H4 + H2', [ETAHNE, ETHYLENE, H2], [-1, 1, 1], [-1, 1, 1], 137.06780078125, 79432823472428.3, 297.2628) </v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="F5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5">
+        <v>-1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5">
+        <v>13.9</v>
+      </c>
+      <c r="Q5">
+        <f>10^P5</f>
+        <v>79432823472428.328</v>
+      </c>
+      <c r="R5">
+        <v>71</v>
+      </c>
+      <c r="S5">
+        <f>R5*4.1868</f>
+        <v>297.26279999999997</v>
+      </c>
+      <c r="T5">
+        <f>S5*1000</f>
+        <v>297262.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>CONCATENATE("Reaction('",F6,"', ",
+"[",G6,", ",H6,IF(COUNTA(G6:J6)=2,"]",IF(COUNTA(G6:J6)=3,CONCATENATE(", ",I6,"], "),IF(COUNTA(G6:J6)=4,CONCATENATE(", ",I6,", ",J6,"], "),NA()))),
+"[",K6,", ",L6,IF(COUNTA(G6:J6)=2,"]",IF(COUNTA(G6:J6)=3,CONCATENATE(", ",M6,"], "),IF(COUNTA(G6:J6)=4,CONCATENATE(", ",M6,", ",N6,"], "),NA()))),
+"[",K6,", ",L6,IF(COUNTA(G6:J6)=2,"]",IF(COUNTA(G6:J6)=3,CONCATENATE(", ",M6,"], "),IF(COUNTA(G6:J6)=4,CONCATENATE(", ",M6,", ",N6,"], "),NA()))),
+O6,", ",
+REPLACE(Q6,FIND(",",Q6),1,"."),", ",
+REPLACE(S6,FIND(",",S6),1,"."),") "
+)</f>
+        <v xml:space="preserve">Reaction('C3H8 --&gt; C3H6 + H2', [PROPANE, PROPYLENE, H2], [-1, 1, 1], [-1, 1, 1], 0, 50118723362727.3, 293.076) </v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6">
+        <v>-1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>13.7</v>
+      </c>
+      <c r="Q6">
+        <f>10^P6</f>
+        <v>50118723362727.258</v>
+      </c>
+      <c r="R6">
+        <v>70</v>
+      </c>
+      <c r="S6">
+        <f>R6*4.1868</f>
+        <v>293.07599999999996</v>
+      </c>
+      <c r="T6">
+        <f>S6*1000</f>
+        <v>293075.99999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>CONCATENATE("Reaction('",F7,"', ",
+"[",G7,", ",H7,IF(COUNTA(G7:J7)=2,"]",IF(COUNTA(G7:J7)=3,CONCATENATE(", ",I7,"], "),IF(COUNTA(G7:J7)=4,CONCATENATE(", ",I7,", ",J7,"], "),NA()))),
+"[",K7,", ",L7,IF(COUNTA(G7:J7)=2,"]",IF(COUNTA(G7:J7)=3,CONCATENATE(", ",M7,"], "),IF(COUNTA(G7:J7)=4,CONCATENATE(", ",M7,", ",N7,"], "),NA()))),
+"[",K7,", ",L7,IF(COUNTA(G7:J7)=2,"]",IF(COUNTA(G7:J7)=3,CONCATENATE(", ",M7,"], "),IF(COUNTA(G7:J7)=4,CONCATENATE(", ",M7,", ",N7,"], "),NA()))),
+O7,", ",
+REPLACE(Q7,FIND(",",Q7),1,"."),", ",
+REPLACE(S7,FIND(",",S7),1,"."),") "
+)</f>
+        <v xml:space="preserve">Reaction('C2H4 + H2 --&gt; C2H6', [ETHYLENE`, H2, ETHANE], [-1, -1, 1], [-1, -1, 1], 0, 794328234.724285, 159.0984) </v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7">
+        <v>-1</v>
+      </c>
+      <c r="L7">
+        <v>-1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>8.9</v>
+      </c>
+      <c r="Q7">
+        <f>10^P7</f>
+        <v>794328234.72428453</v>
+      </c>
+      <c r="R7">
+        <v>38</v>
+      </c>
+      <c r="S7">
+        <f>R7*4.1868</f>
+        <v>159.0984</v>
+      </c>
+      <c r="T7">
+        <f>S7*1000</f>
+        <v>159098.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>CONCATENATE("Reaction('",F8,"', ",
+"[",G8,", ",H8,IF(COUNTA(G8:J8)=2,"]",IF(COUNTA(G8:J8)=3,CONCATENATE(", ",I8,"], "),IF(COUNTA(G8:J8)=4,CONCATENATE(", ",I8,", ",J8,"], "),NA()))),
+"[",K8,", ",L8,IF(COUNTA(G8:J8)=2,"]",IF(COUNTA(G8:J8)=3,CONCATENATE(", ",M8,"], "),IF(COUNTA(G8:J8)=4,CONCATENATE(", ",M8,", ",N8,"], "),NA()))),
+"[",K8,", ",L8,IF(COUNTA(G8:J8)=2,"]",IF(COUNTA(G8:J8)=3,CONCATENATE(", ",M8,"], "),IF(COUNTA(G8:J8)=4,CONCATENATE(", ",M8,", ",N8,"], "),NA()))),
+O8,", ",
+REPLACE(Q8,FIND(",",Q8),1,"."),", ",
+REPLACE(S8,FIND(",",S8),1,"."),") "
+)</f>
+        <v xml:space="preserve">Reaction('C3H6 + H2 --&gt; C3H8', [PROPYLENE, H2, PROPANE], [-1, -1, 1], [-1, -1, 1], 0, 794328234.724285, 159.0984) </v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8">
+        <v>-1</v>
+      </c>
+      <c r="L8">
+        <v>-1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>8.9</v>
+      </c>
+      <c r="Q8">
+        <f>10^P8</f>
+        <v>794328234.72428453</v>
+      </c>
+      <c r="R8">
+        <v>38</v>
+      </c>
+      <c r="S8">
+        <f>R8*4.1868</f>
+        <v>159.0984</v>
+      </c>
+      <c r="T8">
+        <f>S8*1000</f>
+        <v>159098.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>CONCATENATE("Reaction('",F9,"', ",
+"[",G9,", ",H9,IF(COUNTA(G9:J9)=2,"]",IF(COUNTA(G9:J9)=3,CONCATENATE(", ",I9,"], "),IF(COUNTA(G9:J9)=4,CONCATENATE(", ",I9,", ",J9,"], "),NA()))),
+"[",K9,", ",L9,IF(COUNTA(G9:J9)=2,"]",IF(COUNTA(G9:J9)=3,CONCATENATE(", ",M9,"], "),IF(COUNTA(G9:J9)=4,CONCATENATE(", ",M9,", ",N9,"], "),NA()))),
+"[",K9,", ",L9,IF(COUNTA(G9:J9)=2,"]",IF(COUNTA(G9:J9)=3,CONCATENATE(", ",M9,"], "),IF(COUNTA(G9:J9)=4,CONCATENATE(", ",M9,", ",N9,"], "),NA()))),
+O9,", ",
+IFERROR(REPLACE(Q9,FIND(",",Q9),1,"."),Q9),", ",
+REPLACE(S9,FIND(",",S9),1,"."),") "
+)</f>
+        <v xml:space="preserve">Reaction('C2H6 --&gt; 2 CH3*', [ETHANE, CH3_][-1, 2][-1, 2]0, 109647819614319000, 372.6252) </v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="F9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9">
+        <v>-1</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>17.04</v>
+      </c>
+      <c r="Q9">
+        <f>10^P9</f>
+        <v>1.0964781961431858E+17</v>
+      </c>
+      <c r="R9">
+        <v>89</v>
+      </c>
+      <c r="S9">
+        <f>R9*4.1868</f>
+        <v>372.62520000000001</v>
+      </c>
+      <c r="T9">
+        <f>S9*1000</f>
+        <v>372625.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>CONCATENATE("Reaction('",F10,"', ",
+"[",G10,", ",H10,IF(COUNTA(G10:J10)=2,"]",IF(COUNTA(G10:J10)=3,CONCATENATE(", ",I10,"], "),IF(COUNTA(G10:J10)=4,CONCATENATE(", ",I10,", ",J10,"], "),NA()))),
+"[",K10,", ",L10,IF(COUNTA(G10:J10)=2,"]",IF(COUNTA(G10:J10)=3,CONCATENATE(", ",M10,"], "),IF(COUNTA(G10:J10)=4,CONCATENATE(", ",M10,", ",N10,"], "),NA()))),
+"[",K10,", ",L10,IF(COUNTA(G10:J10)=2,"]",IF(COUNTA(G10:J10)=3,CONCATENATE(", ",M10,"], "),IF(COUNTA(G10:J10)=4,CONCATENATE(", ",M10,", ",N10,"], "),NA()))),
+O10,", ",
+IFERROR(REPLACE(Q10,FIND(",",Q10),1,"."),Q10),", ",
+REPLACE(S10,FIND(",",S10),1,"."),") "
+)</f>
+        <v xml:space="preserve">Reaction('C3H8 --&gt;  CH3* + C2H5*', [PROPANE, CH3_, C2H5_], [-1, 1, 1], [-1, 1, 1], 0, 70794578438414500, 360.0648) </v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10">
+        <v>-1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="Q10">
+        <f>10^P10</f>
+        <v>7.0794578438414472E+16</v>
+      </c>
+      <c r="R10">
+        <v>86</v>
+      </c>
+      <c r="S10">
+        <f>R10*4.1868</f>
+        <v>360.06479999999999</v>
+      </c>
+      <c r="T10">
+        <f>S10*1000</f>
+        <v>360064.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>CONCATENATE("Reaction('",F11,"', ",
+"[",G11,", ",H11,IF(COUNTA(G11:J11)=2,"]",IF(COUNTA(G11:J11)=3,CONCATENATE(", ",I11,"], "),IF(COUNTA(G11:J11)=4,CONCATENATE(", ",I11,", ",J11,"], "),NA()))),
+"[",K11,", ",L11,IF(COUNTA(G11:J11)=2,"]",IF(COUNTA(G11:J11)=3,CONCATENATE(", ",M11,"], "),IF(COUNTA(G11:J11)=4,CONCATENATE(", ",M11,", ",N11,"], "),NA()))),
+"[",K11,", ",L11,IF(COUNTA(G11:J11)=2,"]",IF(COUNTA(G11:J11)=3,CONCATENATE(", ",M11,"], "),IF(COUNTA(G11:J11)=4,CONCATENATE(", ",M11,", ",N11,"], "),NA()))),
+O11,", ",
+IFERROR(REPLACE(Q11,FIND(",",Q11),1,"."),Q11),", ",
+REPLACE(S11,FIND(",",S11),1,"."),") "
+)</f>
+        <v xml:space="preserve">Reaction('CH3* + H2 --&gt; C2H4 + H*', [CH3_, H2, METHANE, H_], [-1, -1, 1, 1], [-1, -1, 1, 1], 0, 1513561248.43621, 49.82292) </v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11">
+        <v>-1</v>
+      </c>
+      <c r="L11">
+        <v>-1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>9.18</v>
+      </c>
+      <c r="Q11">
+        <f>10^P11</f>
+        <v>1513561248.4362099</v>
+      </c>
+      <c r="R11">
+        <v>11.9</v>
+      </c>
+      <c r="S11">
+        <f>R11*4.1868</f>
+        <v>49.822919999999996</v>
+      </c>
+      <c r="T11">
+        <f>S11*1000</f>
+        <v>49822.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -601,9 +1057,9 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -638,7 +1094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -705,7 +1161,7 @@
         <v>[14.20512086, 30.24027897, 844.31, 20.58015668, 2482.7, 298.15, 1500]</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -772,7 +1228,7 @@
         <v>[6.596207127, 2.283366772, 2466, 0.8980605713, 567.6, 250, 1500]</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -839,7 +1295,7 @@
         <v>[10.570364, 20.23908474, 872.24, 16.03372504, 2430.4, 298.15, 1500]</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
have no idea what is going on'
</commit_message>
<xml_diff>
--- a/dente_kinetics.xlsx
+++ b/dente_kinetics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\YandexDisk\2. Workplaces\0.1 Tomsk Polytech\02. Reactor Models\Reference Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Projects\SteamCracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>E</t>
   </si>
@@ -109,13 +109,33 @@
   </si>
   <si>
     <t>137.06780078125</t>
+  </si>
+  <si>
+    <t>terrasug</t>
+  </si>
+  <si>
+    <t>C3H8 --&gt; CH3* + C2H5*</t>
+  </si>
+  <si>
+    <t>dente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,14 +162,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S10"/>
+  <dimension ref="B2:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,8 +597,61 @@
         <v>159098.4</v>
       </c>
     </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="N9">
+        <f>10^M9</f>
+        <v>7.0794578438414472E+16</v>
+      </c>
+      <c r="O9">
+        <v>86</v>
+      </c>
+    </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B10" t="str">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="N11">
+        <f>10^M11</f>
+        <v>1.2589254117941763E+17</v>
+      </c>
+      <c r="O11">
+        <f>84000/1000</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="N12">
+        <f>EXP(M11)</f>
+        <v>26695351.310742743</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="P13" s="1">
+        <f>(N9-N11)/N11</f>
+        <v>-0.43765867480964959</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
         <f>CONCATENATE("Reaction('",B5,"', ",
 "[",D5,", ",E5,IF(COUNTA(D5:G5)=2,"]",IF(COUNTA(D5:G5)=3,CONCATENATE(", ",F5,"], "),IF(COUNTA(D5:G5)=4,CONCATENATE(", ",F5,", ",G5,"], "),NA()))),
 "[",H5,", ",I5,IF(COUNTA(D5:G5)=2,"]",IF(COUNTA(D5:G5)=3,CONCATENATE(", ",J5,"], "),IF(COUNTA(D5:G5)=4,CONCATENATE(", ",J5,", ",K5,"], "),NA()))),

</xml_diff>